<commit_message>
update kbv corona report (last time)
</commit_message>
<xml_diff>
--- a/data/kbvreport_export/faktenblatttabellen_2022-12-11.xlsx
+++ b/data/kbvreport_export/faktenblatttabellen_2022-12-11.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="383">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="385">
   <si>
     <t xml:space="preserve">Geimpfte Personen</t>
   </si>
@@ -30,7 +30,7 @@
     <t xml:space="preserve">Vorwoche</t>
   </si>
   <si>
-    <t xml:space="preserve">Stand 15.12.</t>
+    <t xml:space="preserve">Stand 16.12.</t>
   </si>
   <si>
     <t xml:space="preserve">Anteil_Veraenderung</t>
@@ -45,7 +45,7 @@
     <t xml:space="preserve">Gesamt</t>
   </si>
   <si>
-    <t xml:space="preserve">64826202 (77,9 %)</t>
+    <t xml:space="preserve">64826726 (77,9 %)</t>
   </si>
   <si>
     <t xml:space="preserve">64828598 (78,0 %)</t>
@@ -57,7 +57,7 @@
     <t xml:space="preserve">Nicht vollst. geimpft</t>
   </si>
   <si>
-    <t xml:space="preserve">3607334 ( 4,3 %)</t>
+    <t xml:space="preserve">3607319 ( 4,3 %)</t>
   </si>
   <si>
     <t xml:space="preserve">3607059 ( 4,3 %)</t>
@@ -66,7 +66,7 @@
     <t xml:space="preserve">Vollst. geimpft</t>
   </si>
   <si>
-    <t xml:space="preserve">61218868 (73,6 %)</t>
+    <t xml:space="preserve">61219407 (73,6 %)</t>
   </si>
   <si>
     <t xml:space="preserve">61221539 (73,6 %)</t>
@@ -75,7 +75,7 @@
     <t xml:space="preserve">Zusätzl. Booster-Impfung</t>
   </si>
   <si>
-    <t xml:space="preserve">52037774 (62,6 %)</t>
+    <t xml:space="preserve">52041509 (62,6 %)</t>
   </si>
   <si>
     <t xml:space="preserve">52052376 (62,6 %)</t>
@@ -84,7 +84,7 @@
     <t xml:space="preserve">Zusätzl. 2. Booster-Impfung</t>
   </si>
   <si>
-    <t xml:space="preserve">11865816 (14,3 %)</t>
+    <t xml:space="preserve">11916325 (14,3 %)</t>
   </si>
   <si>
     <t xml:space="preserve">12053092 (14,5 %)</t>
@@ -372,7 +372,7 @@
     <t xml:space="preserve">Biontech/Pfizer</t>
   </si>
   <si>
-    <t xml:space="preserve">142519201 (74,7 %)</t>
+    <t xml:space="preserve">142590725 (74,7 %)</t>
   </si>
   <si>
     <t xml:space="preserve">142787126 (74,7 %)</t>
@@ -381,7 +381,7 @@
     <t xml:space="preserve">Impfungen Original</t>
   </si>
   <si>
-    <t xml:space="preserve">138035704</t>
+    <t xml:space="preserve">138041844</t>
   </si>
   <si>
     <t xml:space="preserve">138058384</t>
@@ -390,7 +390,7 @@
     <t xml:space="preserve">Impfungen Omikron</t>
   </si>
   <si>
-    <t xml:space="preserve">4483497</t>
+    <t xml:space="preserve">4548881</t>
   </si>
   <si>
     <t xml:space="preserve">4728742</t>
@@ -417,19 +417,19 @@
     <t xml:space="preserve">Moderna</t>
   </si>
   <si>
-    <t xml:space="preserve">31645776 (16,6 %)</t>
+    <t xml:space="preserve">31646835 (16,6 %)</t>
   </si>
   <si>
     <t xml:space="preserve">31651347 (16,6 %)</t>
   </si>
   <si>
-    <t xml:space="preserve">31562940</t>
+    <t xml:space="preserve">31563105</t>
   </si>
   <si>
     <t xml:space="preserve">31563708</t>
   </si>
   <si>
-    <t xml:space="preserve">82836</t>
+    <t xml:space="preserve">83730</t>
   </si>
   <si>
     <t xml:space="preserve">87639</t>
@@ -465,7 +465,7 @@
     <t xml:space="preserve">Johnson&amp;Johnson</t>
   </si>
   <si>
-    <t xml:space="preserve">3758805 ( 2,0 %)</t>
+    <t xml:space="preserve">3758859 ( 2,0 %)</t>
   </si>
   <si>
     <t xml:space="preserve">3759065 ( 2,0 %)</t>
@@ -480,7 +480,7 @@
     <t xml:space="preserve">Novavax</t>
   </si>
   <si>
-    <t xml:space="preserve">156293 ( 0,1 %)</t>
+    <t xml:space="preserve">156400 ( 0,1 %)</t>
   </si>
   <si>
     <t xml:space="preserve">156863 ( 0,1 %)</t>
@@ -495,7 +495,7 @@
     <t xml:space="preserve">Valneva</t>
   </si>
   <si>
-    <t xml:space="preserve">4757 ( 0,0 %)</t>
+    <t xml:space="preserve">4816 ( 0,0 %)</t>
   </si>
   <si>
     <t xml:space="preserve">5063 ( 0,0 %)</t>
@@ -573,13 +573,13 @@
     <t xml:space="preserve">Reproduktionszahl R</t>
   </si>
   <si>
-    <t xml:space="preserve"> 1,02</t>
+    <t xml:space="preserve"> 1,03</t>
   </si>
   <si>
     <t xml:space="preserve"> 1,09</t>
   </si>
   <si>
-    <t xml:space="preserve">  6,9 %</t>
+    <t xml:space="preserve">  5,8 %</t>
   </si>
   <si>
     <t xml:space="preserve">Neue Fälle je 100.000 EW in 7 Tagen bezogen auf die jeweilige Gruppe:</t>
@@ -609,13 +609,13 @@
     <t xml:space="preserve">- Davon 5-bis-14-Jährige</t>
   </si>
   <si>
-    <t xml:space="preserve">108</t>
+    <t xml:space="preserve">109</t>
   </si>
   <si>
     <t xml:space="preserve">83</t>
   </si>
   <si>
-    <t xml:space="preserve">-23,1 %</t>
+    <t xml:space="preserve">-23,9 %</t>
   </si>
   <si>
     <t xml:space="preserve">- Davon 15-bis-34-Jährige</t>
@@ -624,10 +624,10 @@
     <t xml:space="preserve">226</t>
   </si>
   <si>
-    <t xml:space="preserve">242</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  7,1 %</t>
+    <t xml:space="preserve">243</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  7,5 %</t>
   </si>
   <si>
     <t xml:space="preserve">- Davon 35-bis-59-Jährige</t>
@@ -657,118 +657,118 @@
     <t xml:space="preserve">253</t>
   </si>
   <si>
-    <t xml:space="preserve">294</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 16,2 %</t>
+    <t xml:space="preserve">295</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 16,6 %</t>
   </si>
   <si>
     <t xml:space="preserve">Neue hospitalisierte Fälle je 100.000 EW in 7 Tagen:</t>
   </si>
   <si>
-    <t xml:space="preserve">10,39</t>
-  </si>
-  <si>
-    <t xml:space="preserve">11,20</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  7,8 %</t>
+    <t xml:space="preserve">10,45</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11,52</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 10,2 %</t>
   </si>
   <si>
     <t xml:space="preserve">- Davon über 80-Jährige</t>
   </si>
   <si>
-    <t xml:space="preserve">61,26</t>
-  </si>
-  <si>
-    <t xml:space="preserve">68,25</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 11,4 %</t>
+    <t xml:space="preserve">61,72</t>
+  </si>
+  <si>
+    <t xml:space="preserve">70,29</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 13,9 %</t>
   </si>
   <si>
     <t xml:space="preserve">Hospitalisierungen</t>
   </si>
   <si>
-    <t xml:space="preserve">KW 46</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7243 ( 3,6%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6658 ( 3,9%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> -8,1 %</t>
+    <t xml:space="preserve">KW 47</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6753 ( 4,0%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7376 ( 4,3%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  9,2 %</t>
   </si>
   <si>
     <t xml:space="preserve">Davon unter 4-Jährige</t>
   </si>
   <si>
-    <t xml:space="preserve">140 ( 6,9%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">140 ( 7,8%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  0,0 %</t>
+    <t xml:space="preserve">141 ( 7,9%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">110 ( 7,3%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-22,0 %</t>
   </si>
   <si>
     <t xml:space="preserve">Davon 5- bis 14-Jährige</t>
   </si>
   <si>
-    <t xml:space="preserve">41 ( 0,4%)</t>
-  </si>
-  <si>
     <t xml:space="preserve">46 ( 0,5%)</t>
   </si>
   <si>
-    <t xml:space="preserve"> 12,2 %</t>
+    <t xml:space="preserve">54 ( 0,6%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 17,4 %</t>
   </si>
   <si>
     <t xml:space="preserve">Davon 15- bis 34-Jährige</t>
   </si>
   <si>
-    <t xml:space="preserve">366 ( 0,8%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">397 ( 1,0%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  8,5 %</t>
+    <t xml:space="preserve">401 ( 1,0%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">408 ( 1,0%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  1,7 %</t>
   </si>
   <si>
     <t xml:space="preserve">Davon 35- bis 59-Jährige</t>
   </si>
   <si>
-    <t xml:space="preserve">949 ( 1,1%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">910 ( 1,2%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> -4,1 %</t>
+    <t xml:space="preserve">927 ( 1,2%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">983 ( 1,3%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  6,0 %</t>
   </si>
   <si>
     <t xml:space="preserve">Davon 60- bis 79-Jährige</t>
   </si>
   <si>
-    <t xml:space="preserve">2592 ( 6,6%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2299 ( 7,3%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-11,3 %</t>
+    <t xml:space="preserve">2326 ( 7,3%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2622 ( 8,4%)</t>
   </si>
   <si>
     <t xml:space="preserve">Davon über 80-Jährige</t>
   </si>
   <si>
-    <t xml:space="preserve">3155 (22,2%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2866 (24,3%)</t>
+    <t xml:space="preserve">2912 (24,7%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3199 (24,9%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  9,9 %</t>
   </si>
   <si>
     <t xml:space="preserve">Intensivbetten</t>
@@ -835,34 +835,34 @@
     <t xml:space="preserve">60 bis 79 Jahre</t>
   </si>
   <si>
-    <t xml:space="preserve">146 ( 0,3%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">141 ( 0,4%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> -3,4%</t>
+    <t xml:space="preserve">148 ( 0,3%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">145 ( 0,4%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -2,0%</t>
   </si>
   <si>
     <t xml:space="preserve">80 Jahre +</t>
   </si>
   <si>
-    <t xml:space="preserve">398 ( 2,4%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">310 ( 2,2%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-22,1%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">560 ( 0,2%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">472 ( 0,2%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-15,7%</t>
+    <t xml:space="preserve">400 ( 2,4%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">316 ( 2,2%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-21,0%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">564 ( 0,2%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">482 ( 0,2%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-14,5%</t>
   </si>
   <si>
     <t xml:space="preserve">Übersterblichkeit</t>
@@ -916,124 +916,130 @@
     <t xml:space="preserve">44,4 %</t>
   </si>
   <si>
+    <t xml:space="preserve">1,07</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11,5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wird nicht erreicht</t>
+  </si>
+  <si>
+    <t xml:space="preserve">44,5 %</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1,06</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 6,9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">50,1 %</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 9,2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">37,7 %</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16,4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">42,8 %</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1,04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21,4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">42,9 %</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1,13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16,9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">42,6 %</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1,02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12,6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">44,8 %</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1,09</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 7,6</t>
+  </si>
+  <si>
     <t xml:space="preserve">1,05</t>
   </si>
   <si>
-    <t xml:space="preserve">11,2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">wird nicht erreicht</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 6,8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">50,1 %</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1,04</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 8,9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">37,7 %</t>
-  </si>
-  <si>
-    <t xml:space="preserve">15,8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">42,8 %</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20,9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1,09</t>
-  </si>
-  <si>
-    <t xml:space="preserve">16,4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">42,6 %</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0,99</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12,2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">07.12.2023</t>
-  </si>
-  <si>
-    <t xml:space="preserve">44,8 %</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 7,4</t>
+    <t xml:space="preserve">19,9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">46,0 %</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 8,4</t>
   </si>
   <si>
     <t xml:space="preserve">42,7 %</t>
   </si>
   <si>
-    <t xml:space="preserve">1,06</t>
-  </si>
-  <si>
-    <t xml:space="preserve">18,8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">45,9 %</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1,07</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 8,3</t>
+    <t xml:space="preserve">13,9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">41,6 %</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 9,0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">48,1 %</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13,0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">47,1 %</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12,9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1,01</t>
   </si>
   <si>
     <t xml:space="preserve">13,6</t>
   </si>
   <si>
-    <t xml:space="preserve">41,6 %</t>
+    <t xml:space="preserve">39,2 %</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1,11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">19,0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">40,7 %</t>
   </si>
   <si>
     <t xml:space="preserve">1,03</t>
   </si>
   <si>
-    <t xml:space="preserve">48,1 %</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12,9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">47,1 %</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12,6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">13,5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">07.10.2023</t>
-  </si>
-  <si>
-    <t xml:space="preserve">39,2 %</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1,10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">18,7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">40,7 %</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1,01</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12,4</t>
+    <t xml:space="preserve">13,3</t>
   </si>
   <si>
     <t xml:space="preserve">Fälle gesamt</t>
@@ -1648,7 +1654,7 @@
         <v>296</v>
       </c>
       <c r="D2" t="n">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="E2" t="s">
         <v>297</v>
@@ -1665,16 +1671,16 @@
         <v>50</v>
       </c>
       <c r="B3" t="s">
-        <v>295</v>
+        <v>299</v>
       </c>
       <c r="C3" t="s">
-        <v>296</v>
+        <v>300</v>
       </c>
       <c r="D3" t="n">
         <v>170</v>
       </c>
       <c r="E3" t="s">
-        <v>299</v>
+        <v>301</v>
       </c>
       <c r="F3" t="n">
         <v>152</v>
@@ -1688,16 +1694,16 @@
         <v>54</v>
       </c>
       <c r="B4" t="s">
+        <v>302</v>
+      </c>
+      <c r="C4" t="s">
         <v>300</v>
-      </c>
-      <c r="C4" t="s">
-        <v>301</v>
       </c>
       <c r="D4" t="n">
         <v>138</v>
       </c>
       <c r="E4" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="F4" t="n">
         <v>123</v>
@@ -1711,16 +1717,16 @@
         <v>58</v>
       </c>
       <c r="B5" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="C5" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D5" t="n">
         <v>235</v>
       </c>
       <c r="E5" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="F5" t="n">
         <v>247</v>
@@ -1734,16 +1740,16 @@
         <v>62</v>
       </c>
       <c r="B6" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="C6" t="s">
-        <v>296</v>
+        <v>307</v>
       </c>
       <c r="D6" t="n">
         <v>296</v>
       </c>
       <c r="E6" t="s">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="F6" t="n">
         <v>373</v>
@@ -1757,16 +1763,16 @@
         <v>66</v>
       </c>
       <c r="B7" t="s">
-        <v>305</v>
+        <v>309</v>
       </c>
       <c r="C7" t="s">
-        <v>307</v>
+        <v>310</v>
       </c>
       <c r="D7" t="n">
         <v>404</v>
       </c>
       <c r="E7" t="s">
-        <v>308</v>
+        <v>311</v>
       </c>
       <c r="F7" t="n">
         <v>381</v>
@@ -1780,22 +1786,22 @@
         <v>70</v>
       </c>
       <c r="B8" t="s">
-        <v>309</v>
+        <v>312</v>
       </c>
       <c r="C8" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="D8" t="n">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="E8" t="s">
-        <v>311</v>
+        <v>314</v>
       </c>
       <c r="F8" t="n">
         <v>225</v>
       </c>
       <c r="G8" t="s">
-        <v>312</v>
+        <v>298</v>
       </c>
     </row>
     <row r="9">
@@ -1803,16 +1809,16 @@
         <v>74</v>
       </c>
       <c r="B9" t="s">
-        <v>313</v>
+        <v>315</v>
       </c>
       <c r="C9" t="s">
-        <v>296</v>
+        <v>316</v>
       </c>
       <c r="D9" t="n">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="E9" t="s">
-        <v>314</v>
+        <v>317</v>
       </c>
       <c r="F9" t="n">
         <v>191</v>
@@ -1826,16 +1832,16 @@
         <v>78</v>
       </c>
       <c r="B10" t="s">
-        <v>315</v>
+        <v>306</v>
       </c>
       <c r="C10" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="D10" t="n">
         <v>304</v>
       </c>
       <c r="E10" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="F10" t="n">
         <v>389</v>
@@ -1849,19 +1855,19 @@
         <v>81</v>
       </c>
       <c r="B11" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="C11" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="D11" t="n">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="E11" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="F11" t="n">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="G11" t="s">
         <v>298</v>
@@ -1872,19 +1878,19 @@
         <v>85</v>
       </c>
       <c r="B12" t="s">
-        <v>309</v>
+        <v>322</v>
       </c>
       <c r="C12" t="s">
-        <v>296</v>
+        <v>316</v>
       </c>
       <c r="D12" t="n">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="E12" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="F12" t="n">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="G12" t="s">
         <v>298</v>
@@ -1895,16 +1901,16 @@
         <v>89</v>
       </c>
       <c r="B13" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="C13" t="s">
-        <v>323</v>
+        <v>296</v>
       </c>
       <c r="D13" t="n">
         <v>170</v>
       </c>
       <c r="E13" t="s">
-        <v>320</v>
+        <v>325</v>
       </c>
       <c r="F13" t="n">
         <v>168</v>
@@ -1918,16 +1924,16 @@
         <v>93</v>
       </c>
       <c r="B14" t="s">
-        <v>324</v>
+        <v>326</v>
       </c>
       <c r="C14" t="s">
-        <v>296</v>
+        <v>318</v>
       </c>
       <c r="D14" t="n">
         <v>232</v>
       </c>
       <c r="E14" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="F14" t="n">
         <v>226</v>
@@ -1941,19 +1947,19 @@
         <v>97</v>
       </c>
       <c r="B15" t="s">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="C15" t="s">
-        <v>323</v>
+        <v>313</v>
       </c>
       <c r="D15" t="n">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="E15" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="F15" t="n">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="G15" t="s">
         <v>298</v>
@@ -1964,22 +1970,22 @@
         <v>101</v>
       </c>
       <c r="B16" t="s">
-        <v>315</v>
+        <v>322</v>
       </c>
       <c r="C16" t="s">
-        <v>310</v>
+        <v>330</v>
       </c>
       <c r="D16" t="n">
         <v>189</v>
       </c>
       <c r="E16" t="s">
-        <v>328</v>
+        <v>331</v>
       </c>
       <c r="F16" t="n">
         <v>238</v>
       </c>
       <c r="G16" t="s">
-        <v>329</v>
+        <v>298</v>
       </c>
     </row>
     <row r="17">
@@ -1987,16 +1993,16 @@
         <v>105</v>
       </c>
       <c r="B17" t="s">
-        <v>330</v>
+        <v>332</v>
       </c>
       <c r="C17" t="s">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="D17" t="n">
         <v>290</v>
       </c>
       <c r="E17" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
       <c r="F17" t="n">
         <v>302</v>
@@ -2010,19 +2016,19 @@
         <v>109</v>
       </c>
       <c r="B18" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="C18" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="D18" t="n">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="E18" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="F18" t="n">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="G18" t="s">
         <v>298</v>
@@ -2044,354 +2050,354 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>336</v>
+        <v>338</v>
       </c>
       <c r="B1" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="C1" t="s">
-        <v>338</v>
+        <v>340</v>
       </c>
       <c r="D1" t="s">
-        <v>339</v>
+        <v>341</v>
       </c>
       <c r="E1" t="s">
-        <v>340</v>
+        <v>342</v>
       </c>
       <c r="F1" t="s">
-        <v>341</v>
+        <v>343</v>
       </c>
       <c r="G1" t="s">
-        <v>342</v>
+        <v>344</v>
       </c>
       <c r="H1" t="s">
-        <v>343</v>
+        <v>345</v>
       </c>
       <c r="I1" t="s">
-        <v>344</v>
+        <v>346</v>
       </c>
       <c r="J1" t="s">
-        <v>345</v>
+        <v>347</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>346</v>
+        <v>348</v>
       </c>
       <c r="B2" t="s">
-        <v>347</v>
+        <v>349</v>
       </c>
       <c r="C2" t="n">
         <v>5613343</v>
       </c>
       <c r="D2" t="s">
-        <v>348</v>
+        <v>350</v>
       </c>
       <c r="E2" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="F2" t="n">
         <v>118382</v>
       </c>
       <c r="G2" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="H2" t="n">
         <v>1241</v>
       </c>
       <c r="I2" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="J2" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="B3" t="s">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="C3" t="n">
         <v>38598292</v>
       </c>
       <c r="D3" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c r="E3" t="s">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="F3" t="n">
         <v>213508</v>
       </c>
       <c r="G3" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="H3" t="n">
         <v>842</v>
       </c>
       <c r="I3" t="s">
-        <v>356</v>
+        <v>358</v>
       </c>
       <c r="J3" t="s">
-        <v>357</v>
+        <v>359</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>358</v>
+        <v>360</v>
       </c>
       <c r="B4" t="s">
-        <v>359</v>
+        <v>361</v>
       </c>
       <c r="C4" t="n">
         <v>5549479</v>
       </c>
       <c r="D4" t="s">
-        <v>360</v>
+        <v>362</v>
       </c>
       <c r="E4" t="s">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="F4" t="n">
         <v>116422</v>
       </c>
       <c r="G4" t="s">
-        <v>356</v>
+        <v>358</v>
       </c>
       <c r="H4" t="n">
         <v>741</v>
       </c>
       <c r="I4" t="s">
-        <v>361</v>
+        <v>363</v>
       </c>
       <c r="J4" t="s">
-        <v>362</v>
+        <v>364</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="B5" t="s">
-        <v>363</v>
+        <v>365</v>
       </c>
       <c r="C5" t="n">
         <v>5448700</v>
       </c>
       <c r="D5" t="s">
-        <v>356</v>
+        <v>358</v>
       </c>
       <c r="E5" t="s">
-        <v>364</v>
+        <v>366</v>
       </c>
       <c r="F5" t="n">
         <v>182419</v>
       </c>
       <c r="G5" t="s">
-        <v>346</v>
+        <v>348</v>
       </c>
       <c r="H5" t="n">
         <v>734</v>
       </c>
       <c r="I5" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="J5" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>366</v>
+        <v>368</v>
       </c>
       <c r="B6" t="s">
-        <v>367</v>
+        <v>369</v>
       </c>
       <c r="C6" t="n">
         <v>8662418</v>
       </c>
       <c r="D6" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="E6" t="s">
-        <v>368</v>
+        <v>370</v>
       </c>
       <c r="F6" t="n">
         <v>34482</v>
       </c>
       <c r="G6" t="s">
-        <v>361</v>
+        <v>363</v>
       </c>
       <c r="H6" t="n">
         <v>458</v>
       </c>
       <c r="I6" t="s">
-        <v>358</v>
+        <v>360</v>
       </c>
       <c r="J6" t="s">
-        <v>369</v>
+        <v>371</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>361</v>
+        <v>363</v>
       </c>
       <c r="B7" t="s">
-        <v>370</v>
+        <v>372</v>
       </c>
       <c r="C7" t="n">
         <v>36755666</v>
       </c>
       <c r="D7" t="s">
-        <v>358</v>
+        <v>360</v>
       </c>
       <c r="E7" t="s">
-        <v>371</v>
+        <v>373</v>
       </c>
       <c r="F7" t="n">
         <v>25584</v>
       </c>
       <c r="G7" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c r="H7" t="n">
         <v>84</v>
       </c>
       <c r="I7" t="s">
-        <v>360</v>
+        <v>362</v>
       </c>
       <c r="J7" t="s">
-        <v>372</v>
+        <v>374</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>356</v>
+        <v>358</v>
       </c>
       <c r="B8" t="s">
-        <v>373</v>
+        <v>375</v>
       </c>
       <c r="C8" t="n">
         <v>24709404</v>
       </c>
       <c r="D8" t="s">
-        <v>361</v>
+        <v>363</v>
       </c>
       <c r="E8" t="s">
-        <v>374</v>
+        <v>376</v>
       </c>
       <c r="F8" t="n">
         <v>158971</v>
       </c>
       <c r="G8" t="s">
-        <v>360</v>
+        <v>362</v>
       </c>
       <c r="H8" t="n">
         <v>79</v>
       </c>
       <c r="I8" t="s">
-        <v>346</v>
+        <v>348</v>
       </c>
       <c r="J8" t="s">
-        <v>375</v>
+        <v>377</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c r="B9" t="s">
-        <v>376</v>
+        <v>378</v>
       </c>
       <c r="C9" t="n">
         <v>24281498</v>
       </c>
       <c r="D9" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="E9" t="s">
-        <v>374</v>
+        <v>376</v>
       </c>
       <c r="F9" t="n">
         <v>160652</v>
       </c>
       <c r="G9" t="s">
-        <v>358</v>
+        <v>360</v>
       </c>
       <c r="H9" t="n">
         <v>71</v>
       </c>
       <c r="I9" t="s">
-        <v>366</v>
+        <v>368</v>
       </c>
       <c r="J9" t="s">
-        <v>377</v>
+        <v>379</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>360</v>
+        <v>362</v>
       </c>
       <c r="B10" t="s">
-        <v>378</v>
+        <v>380</v>
       </c>
       <c r="C10" t="n">
         <v>13632635</v>
       </c>
       <c r="D10" t="s">
-        <v>346</v>
+        <v>348</v>
       </c>
       <c r="E10" t="s">
-        <v>374</v>
+        <v>376</v>
       </c>
       <c r="F10" t="n">
         <v>21265</v>
       </c>
       <c r="G10" t="s">
-        <v>366</v>
+        <v>368</v>
       </c>
       <c r="H10" t="n">
         <v>68</v>
       </c>
       <c r="I10" t="s">
-        <v>348</v>
+        <v>350</v>
       </c>
       <c r="J10" t="s">
-        <v>379</v>
+        <v>381</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>348</v>
+        <v>350</v>
       </c>
       <c r="B11" t="s">
-        <v>380</v>
+        <v>382</v>
       </c>
       <c r="C11" t="n">
         <v>6357489</v>
       </c>
       <c r="D11" t="s">
-        <v>366</v>
+        <v>368</v>
       </c>
       <c r="E11" t="s">
-        <v>381</v>
+        <v>383</v>
       </c>
       <c r="F11" t="n">
         <v>23641</v>
       </c>
       <c r="G11" t="s">
-        <v>348</v>
+        <v>350</v>
       </c>
       <c r="H11" t="n">
         <v>16</v>
       </c>
       <c r="I11" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c r="J11" t="s">
-        <v>382</v>
+        <v>384</v>
       </c>
     </row>
   </sheetData>
@@ -2535,7 +2541,7 @@
         <v>238</v>
       </c>
       <c r="G2" t="n">
-        <v>232</v>
+        <v>233</v>
       </c>
     </row>
     <row r="3">
@@ -2673,7 +2679,7 @@
         <v>225</v>
       </c>
       <c r="G8" t="n">
-        <v>256</v>
+        <v>257</v>
       </c>
     </row>
     <row r="9">
@@ -2696,7 +2702,7 @@
         <v>191</v>
       </c>
       <c r="G9" t="n">
-        <v>193</v>
+        <v>194</v>
       </c>
     </row>
     <row r="10">
@@ -2739,10 +2745,10 @@
         <v>84</v>
       </c>
       <c r="F11" t="n">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="G11" t="n">
-        <v>426</v>
+        <v>427</v>
       </c>
     </row>
     <row r="12">
@@ -2762,10 +2768,10 @@
         <v>88</v>
       </c>
       <c r="F12" t="n">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="G12" t="n">
-        <v>275</v>
+        <v>276</v>
       </c>
     </row>
     <row r="13">
@@ -2831,10 +2837,10 @@
         <v>100</v>
       </c>
       <c r="F15" t="n">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="G15" t="n">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="16">
@@ -2900,10 +2906,10 @@
         <v>112</v>
       </c>
       <c r="F18" t="n">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="G18" t="n">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
   </sheetData>
@@ -3520,21 +3526,21 @@
         <v>244</v>
       </c>
       <c r="D7" t="s">
-        <v>245</v>
+        <v>208</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
+        <v>245</v>
+      </c>
+      <c r="B8" t="s">
         <v>246</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>247</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>248</v>
-      </c>
-      <c r="D8" t="s">
-        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>